<commit_message>
11월 3주차 진행상황(11/18) commit
</commit_message>
<xml_diff>
--- a/LectureProject_1107/src/main/webapp/WEB-INF/readMe/개발 진행현황_유예원.xlsx
+++ b/LectureProject_1107/src/main/webapp/WEB-INF/readMe/개발 진행현황_유예원.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="88">
   <si>
     <t>대분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -476,6 +476,18 @@
   </si>
   <si>
     <t>관리자 승인/반려 화면 개발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수강신청 리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리스트 화면 페이징 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/addStudy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -754,7 +766,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -851,6 +863,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -871,57 +937,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1470,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M37"/>
+  <dimension ref="B2:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1496,62 +1511,62 @@
       <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="22"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="41" t="s">
+      <c r="D5" s="51"/>
+      <c r="E5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="33" t="s">
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="44" t="s">
+      <c r="M5" s="49" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="43"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="26" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1567,11 +1582,11 @@
       <c r="K6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="34"/>
-      <c r="M6" s="44"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="49"/>
     </row>
     <row r="7" spans="2:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="39" t="s">
         <v>78</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -1600,10 +1615,10 @@
         <v>18</v>
       </c>
       <c r="L7" s="20"/>
-      <c r="M7" s="32"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="46"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="30" t="s">
         <v>19</v>
       </c>
@@ -1632,14 +1647,14 @@
         <v>18</v>
       </c>
       <c r="L8" s="20"/>
-      <c r="M8" s="32"/>
+      <c r="M8" s="50"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="46"/>
-      <c r="C9" s="50" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="42" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="25" t="s">
@@ -1662,12 +1677,12 @@
         <v>28</v>
       </c>
       <c r="L9" s="20"/>
-      <c r="M9" s="32"/>
+      <c r="M9" s="50"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="46"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="49"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="43"/>
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1688,11 +1703,11 @@
         <v>18</v>
       </c>
       <c r="L10" s="20"/>
-      <c r="M10" s="32"/>
+      <c r="M10" s="50"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="46"/>
-      <c r="C11" s="52"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="27" t="s">
         <v>25</v>
       </c>
@@ -1714,10 +1729,10 @@
         <v>27</v>
       </c>
       <c r="L11" s="20"/>
-      <c r="M11" s="32"/>
+      <c r="M11" s="50"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="46"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="27" t="s">
         <v>29</v>
       </c>
@@ -1744,11 +1759,11 @@
         <v>27</v>
       </c>
       <c r="L12" s="20"/>
-      <c r="M12" s="32"/>
+      <c r="M12" s="50"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="46"/>
-      <c r="C13" s="50" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="35" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -1774,11 +1789,11 @@
         <v>27</v>
       </c>
       <c r="L13" s="20"/>
-      <c r="M13" s="32"/>
+      <c r="M13" s="50"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="46"/>
-      <c r="C14" s="52"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="23" t="s">
         <v>35</v>
       </c>
@@ -1802,11 +1817,11 @@
         <v>27</v>
       </c>
       <c r="L14" s="20"/>
-      <c r="M14" s="32"/>
+      <c r="M14" s="50"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="46"/>
-      <c r="C15" s="50" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="35" t="s">
         <v>72</v>
       </c>
       <c r="D15" s="27" t="s">
@@ -1832,11 +1847,11 @@
         <v>27</v>
       </c>
       <c r="L15" s="20"/>
-      <c r="M15" s="32"/>
+      <c r="M15" s="50"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="46"/>
-      <c r="C16" s="52"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="27" t="s">
         <v>73</v>
       </c>
@@ -1860,10 +1875,10 @@
         <v>27</v>
       </c>
       <c r="L16" s="20"/>
-      <c r="M16" s="32"/>
+      <c r="M16" s="50"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="47"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="27" t="s">
         <v>37</v>
       </c>
@@ -1890,7 +1905,7 @@
         <v>27</v>
       </c>
       <c r="L17" s="20"/>
-      <c r="M17" s="32"/>
+      <c r="M17" s="50"/>
     </row>
     <row r="18" spans="2:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
@@ -1904,13 +1919,13 @@
       <c r="J18" s="12"/>
       <c r="K18" s="16"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="32"/>
+      <c r="M18" s="50"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="35" t="s">
         <v>56</v>
       </c>
       <c r="D19" s="29" t="s">
@@ -1938,9 +1953,9 @@
       <c r="L19" s="20"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="53"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="50" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="35" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1963,9 +1978,9 @@
       <c r="L20" s="20"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="53"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="2" t="s">
         <v>61</v>
       </c>
@@ -1986,9 +2001,9 @@
       <c r="L21" s="20"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="53"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="36"/>
       <c r="E22" s="2" t="s">
         <v>62</v>
       </c>
@@ -2009,8 +2024,8 @@
       <c r="L22" s="20"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="53"/>
-      <c r="C23" s="51"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="30" t="s">
         <v>59</v>
       </c>
@@ -2034,8 +2049,8 @@
       <c r="L23" s="20"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="53"/>
-      <c r="C24" s="52"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="30" t="s">
         <v>65</v>
       </c>
@@ -2047,112 +2062,146 @@
         <v>44882</v>
       </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
+      <c r="I24" s="24">
+        <v>44882</v>
+      </c>
+      <c r="J24" s="18">
+        <v>1</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="L24" s="20"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="53"/>
-      <c r="C25" s="30" t="s">
+      <c r="B25" s="34"/>
+      <c r="C25" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>49</v>
+      <c r="D25" s="32" t="s">
+        <v>85</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="13">
-        <v>44883</v>
+        <v>44882</v>
       </c>
       <c r="H25" s="9"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+      <c r="I25" s="24">
+        <v>44882</v>
+      </c>
+      <c r="J25" s="18">
+        <v>1</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="L25" s="20"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="53"/>
-      <c r="C26" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>55</v>
+      <c r="B26" s="34"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="13">
         <v>44883</v>
       </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="24">
+        <v>44883</v>
+      </c>
+      <c r="J26" s="18">
+        <v>1</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="L26" s="20"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="53"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>55</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="G27" s="13">
         <v>44883</v>
       </c>
       <c r="H27" s="10"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
+      <c r="I27" s="24">
+        <v>44883</v>
+      </c>
+      <c r="J27" s="18">
+        <v>1</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="L27" s="20"/>
     </row>
-    <row r="28" spans="2:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="5"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="21"/>
-    </row>
-    <row r="29" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="53" t="s">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="34"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="13">
+        <v>44883</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="24">
+        <v>44883</v>
+      </c>
+      <c r="J28" s="18">
+        <v>1</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="20"/>
+    </row>
+    <row r="29" spans="2:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="5"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="21"/>
+    </row>
+    <row r="30" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C30" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D30" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E30" s="25" t="s">
         <v>67</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="13">
-        <v>44886</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="20"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="53"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="13">
@@ -2165,17 +2214,15 @@
       <c r="L30" s="20"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="53"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54" t="s">
-        <v>69</v>
-      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="13">
-        <v>44887</v>
+        <v>44886</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="24"/>
@@ -2184,30 +2231,30 @@
       <c r="L31" s="20"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="53"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33" t="s">
+        <v>69</v>
+      </c>
       <c r="E32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="13">
         <v>44887</v>
       </c>
       <c r="H32" s="10"/>
-      <c r="I32" s="13"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
       <c r="L32" s="20"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="50" t="s">
-        <v>63</v>
-      </c>
+      <c r="B33" s="34"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="13">
@@ -2219,37 +2266,35 @@
       <c r="K33" s="18"/>
       <c r="L33" s="20"/>
     </row>
-    <row r="34" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="53"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="52"/>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="34"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="35" t="s">
+        <v>63</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="13">
         <v>44887</v>
       </c>
       <c r="H34" s="10"/>
-      <c r="I34" s="24"/>
+      <c r="I34" s="13"/>
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
       <c r="L34" s="20"/>
     </row>
     <row r="35" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="53"/>
-      <c r="C35" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>76</v>
-      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="13">
-        <v>44888</v>
+        <v>44887</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="24"/>
@@ -2257,13 +2302,26 @@
       <c r="K35" s="18"/>
       <c r="L35" s="20"/>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="F36" s="1"/>
-      <c r="G36"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="17"/>
-      <c r="K36" s="19"/>
-      <c r="L36"/>
+    <row r="36" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="34"/>
+      <c r="C36" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="13">
+        <v>44888</v>
+      </c>
+      <c r="H36" s="10"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="20"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F37" s="1"/>
@@ -2273,36 +2331,45 @@
       <c r="K37" s="19"/>
       <c r="L37"/>
     </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F38" s="1"/>
+      <c r="G38"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="17"/>
+      <c r="K38" s="19"/>
+      <c r="L38"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D20:D22"/>
+  <mergeCells count="26">
+    <mergeCell ref="M7:M18"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="M5:M6"/>
     <mergeCell ref="B7:B17"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M7:M18"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C30:C35"/>
+    <mergeCell ref="B30:B36"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J23:J27 J7:J17">
+  <conditionalFormatting sqref="J7:J17 J23:J28">
     <cfRule type="cellIs" dxfId="25" priority="101" operator="equal">
       <formula>0.5</formula>
     </cfRule>
@@ -2310,7 +2377,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K4 K38:K1048576 J36:J37 K7:K27">
+  <conditionalFormatting sqref="K1:K4 K39:K1048576 J37:J38 K7:K28">
     <cfRule type="cellIs" dxfId="23" priority="99" operator="equal">
       <formula>"진행중"</formula>
     </cfRule>
@@ -2326,7 +2393,7 @@
       <formula>"완료"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
+  <conditionalFormatting sqref="K29">
     <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"진행중"</formula>
     </cfRule>
@@ -2334,7 +2401,7 @@
       <formula>"완료"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J31">
+  <conditionalFormatting sqref="J30:J32">
     <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>0.5</formula>
     </cfRule>
@@ -2342,7 +2409,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29:K31">
+  <conditionalFormatting sqref="K30:K32">
     <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"진행중"</formula>
     </cfRule>
@@ -2358,7 +2425,7 @@
       <formula>"완료"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32:K33">
+  <conditionalFormatting sqref="K33:K34">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"진행중"</formula>
     </cfRule>
@@ -2366,7 +2433,7 @@
       <formula>"완료"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32:J33">
+  <conditionalFormatting sqref="J33:J34">
     <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>0.5</formula>
     </cfRule>
@@ -2374,7 +2441,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
+  <conditionalFormatting sqref="K35">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"진행중"</formula>
     </cfRule>
@@ -2382,7 +2449,7 @@
       <formula>"완료"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+  <conditionalFormatting sqref="J35">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>0.5</formula>
     </cfRule>
@@ -2390,7 +2457,7 @@
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
+  <conditionalFormatting sqref="K36">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"진행중"</formula>
     </cfRule>
@@ -2398,7 +2465,7 @@
       <formula>"완료"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
+  <conditionalFormatting sqref="J36">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0.5</formula>
     </cfRule>

</xml_diff>